<commit_message>
Se corrigieron detalles de las plantillas
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Ciclo de vida IWM/Capacitación/PTLL_Evaluacion_capacitacion.xlsx
+++ b/Organización/Procesos/Ciclo de vida IWM/Capacitación/PTLL_Evaluacion_capacitacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Documents\IWM\CMMI3\Repositorio\Organización\Procesos\Ciclo de vida IWM\Capacitación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Procesos\Ciclo de vida IWM\Capacitación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -69,9 +69,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0%"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -285,6 +282,12 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -294,21 +297,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -318,7 +315,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -604,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,23 +611,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -640,7 +637,7 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -664,28 +661,28 @@
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
-      <c r="J3" s="17">
-        <f>(B3+C3+D3+E3+F3+G3+H3+I3)/8</f>
-        <v>0</v>
+      <c r="J3" s="17" t="e">
+        <f>SUM(B3:I4)/COUNTIF(B3:I4,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="16"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
       <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,23 +697,23 @@
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="17">
-        <f t="shared" ref="J5" si="0">(B5+C5+D5+E5+F5+G5+H5+I5)/8</f>
-        <v>0</v>
+      <c r="J5" s="17" t="e">
+        <f t="shared" ref="J5" si="0">SUM(B5:I6)/COUNTIF(B5:I6,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -731,23 +728,23 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="17">
-        <f t="shared" ref="J7" si="1">(B7+C7+D7+E7+F7+G7+H7+I7)/8</f>
-        <v>0</v>
+      <c r="J7" s="17" t="e">
+        <f t="shared" ref="J7" si="1">SUM(B7:I8)/COUNTIF(B7:I8,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -762,23 +759,23 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="17">
-        <f t="shared" ref="J9" si="2">(B9+C9+D9+E9+F9+G9+H9+I9)/8</f>
-        <v>0</v>
+      <c r="J9" s="17" t="e">
+        <f t="shared" ref="J9" si="2">SUM(B9:I10)/COUNTIF(B9:I10,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -793,23 +790,23 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="17">
-        <f t="shared" ref="J11" si="3">(B11+C11+D11+E11+F11+G11+H11+I11)/8</f>
-        <v>0</v>
+      <c r="J11" s="17" t="e">
+        <f t="shared" ref="J11" si="3">SUM(B11:I12)/COUNTIF(B11:I12,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -824,23 +821,23 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="17">
-        <f t="shared" ref="J13" si="4">(B13+C13+D13+E13+F13+G13+H13+I13)/8</f>
-        <v>0</v>
+      <c r="J13" s="17" t="e">
+        <f t="shared" ref="J13" si="4">SUM(B13:I14)/COUNTIF(B13:I14,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -855,23 +852,23 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="17">
-        <f t="shared" ref="J15" si="5">(B15+C15+D15+E15+F15+G15+H15+I15)/8</f>
-        <v>0</v>
+      <c r="J15" s="17" t="e">
+        <f t="shared" ref="J15" si="5">SUM(B15:I16)/COUNTIF(B15:I16,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -886,23 +883,23 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
-      <c r="J17" s="17">
-        <f t="shared" ref="J17" si="6">(B17+C17+D17+E17+F17+G17+H17+I17)/8</f>
-        <v>0</v>
+      <c r="J17" s="17" t="e">
+        <f t="shared" ref="J17" si="6">SUM(B17:I18)/COUNTIF(B17:I18,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
       <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -917,23 +914,23 @@
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
-      <c r="J19" s="17">
-        <f t="shared" ref="J19" si="7">(B19+C19+D19+E19+F19+G19+H19+I19)/8</f>
-        <v>0</v>
+      <c r="J19" s="17" t="e">
+        <f t="shared" ref="J19" si="7">SUM(B19:I20)/COUNTIF(B19:I20,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -948,23 +945,23 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
-      <c r="J21" s="17">
-        <f t="shared" ref="J21" si="8">(B21+C21+D21+E21+F21+G21+H21+I21)/8</f>
-        <v>0</v>
+      <c r="J21" s="17" t="e">
+        <f t="shared" ref="J21" si="8">SUM(B21:I22)/COUNTIF(B21:I22,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
       <c r="J22" s="18"/>
     </row>
     <row r="23" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -979,23 +976,23 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
-      <c r="J23" s="17">
-        <f>(B23+C23+D23+E23+F23+G23+H23+I23)/8</f>
-        <v>0</v>
+      <c r="J23" s="17" t="e">
+        <f t="shared" ref="J23" si="9">SUM(B23:I24)/COUNTIF(B23:I24,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
       <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1005,14 +1002,14 @@
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="11"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="19">
-        <f>(J23+J21+J19+J17+J15+J13+J11+J9+J7+J5+J3)/55</f>
-        <v>0</v>
+      <c r="J25" s="19" t="e">
+        <f>SUM(J3:J24)/COUNTIF(J3:J24,"&lt;&gt;")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1041,6 @@
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="J15:J16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
@@ -1054,8 +1050,6 @@
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
@@ -1064,6 +1058,7 @@
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
@@ -1080,7 +1075,8 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
@@ -1090,8 +1086,6 @@
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
@@ -1100,9 +1094,7 @@
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J7:J8"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
@@ -1110,6 +1102,8 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:J1"/>
@@ -1119,6 +1113,9 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>